<commit_message>
modify domain name in config file
</commit_message>
<xml_diff>
--- a/assets/Approved_Guests.xlsx
+++ b/assets/Approved_Guests.xlsx
@@ -464,11 +464,11 @@
         <v>558723345</v>
       </c>
       <c r="D2" t="n">
-        <v>884417</v>
+        <v>582050</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/884417</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/582050</t>
         </is>
       </c>
     </row>
@@ -487,11 +487,11 @@
         <v>562374345</v>
       </c>
       <c r="D3" t="n">
-        <v>574204</v>
+        <v>578600</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/574204</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/578600</t>
         </is>
       </c>
     </row>
@@ -510,11 +510,11 @@
         <v>264427892</v>
       </c>
       <c r="D4" t="n">
-        <v>797692</v>
+        <v>322289</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/797692</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/322289</t>
         </is>
       </c>
     </row>
@@ -533,11 +533,11 @@
         <v>246402004</v>
       </c>
       <c r="D5" t="n">
-        <v>352246</v>
+        <v>894139</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/352246</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/894139</t>
         </is>
       </c>
     </row>
@@ -556,11 +556,11 @@
         <v>597892321</v>
       </c>
       <c r="D6" t="n">
-        <v>640319</v>
+        <v>718113</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/640319</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/718113</t>
         </is>
       </c>
     </row>
@@ -579,11 +579,11 @@
         <v>244345678</v>
       </c>
       <c r="D7" t="n">
-        <v>231535</v>
+        <v>185950</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/231535</t>
+          <t>https://8000-gaius1-qrcodeticketings-256zdob18db.ws-eu63.gitpod.io/ticket/185950</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
generate digital ticket for each guest
</commit_message>
<xml_diff>
--- a/assets/Approved_Guests.xlsx
+++ b/assets/Approved_Guests.xlsx
@@ -1,39 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,22 +44,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -355,52 +406,279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125" style="1" customWidth="1"/>
+    <col width="11.5703125" customWidth="1" style="1" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1"/>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>phone_number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ticket_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ticket_link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jephtali Ashong</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0504281298</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>440938</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/440938</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Paulyn</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0245438155</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>175826</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/175826</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Joshua-Bernard and Akita</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0507631899</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Couple Ticket</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>413334</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/413334</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Naa Shome</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0249747986</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>837572</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/837572</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rebecca Korankye</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0557658645</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>109417</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/109417</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Christabel Quaye</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0549078544</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>483721</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/483721</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evette Arvo-Quardoo </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0551616109</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>487282</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/487282</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lawrence</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0243857169</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Single Ticket</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>929571</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/929571</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" t="n">
+        <v>277370</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/277370</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" t="n">
+        <v>157631</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://93mtzf.deta.dev/ticket/157631</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
generate diginew tal ticket for each guest
</commit_message>
<xml_diff>
--- a/assets/Approved_Guests.xlsx
+++ b/assets/Approved_Guests.xlsx
@@ -466,11 +466,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>440938</v>
+        <v>606323</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/440938</t>
+          <t>https://93mtzf.deta.dev/ticket/606323</t>
         </is>
       </c>
     </row>
@@ -491,11 +491,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>175826</v>
+        <v>503433</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/175826</t>
+          <t>https://93mtzf.deta.dev/ticket/503433</t>
         </is>
       </c>
     </row>
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>413334</v>
+        <v>257987</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/413334</t>
+          <t>https://93mtzf.deta.dev/ticket/257987</t>
         </is>
       </c>
     </row>
@@ -541,11 +541,11 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>837572</v>
+        <v>799241</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/837572</t>
+          <t>https://93mtzf.deta.dev/ticket/799241</t>
         </is>
       </c>
     </row>
@@ -566,11 +566,11 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>109417</v>
+        <v>796294</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/109417</t>
+          <t>https://93mtzf.deta.dev/ticket/796294</t>
         </is>
       </c>
     </row>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>483721</v>
+        <v>184961</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/483721</t>
+          <t>https://93mtzf.deta.dev/ticket/184961</t>
         </is>
       </c>
     </row>
@@ -616,11 +616,11 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>487282</v>
+        <v>502539</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/487282</t>
+          <t>https://93mtzf.deta.dev/ticket/502539</t>
         </is>
       </c>
     </row>
@@ -641,11 +641,11 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>929571</v>
+        <v>929043</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/929571</t>
+          <t>https://93mtzf.deta.dev/ticket/929043</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
generate new digital ticket for each guest
</commit_message>
<xml_diff>
--- a/assets/Approved_Guests.xlsx
+++ b/assets/Approved_Guests.xlsx
@@ -411,7 +411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -466,11 +466,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>606323</v>
+        <v>378918</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/606323</t>
+          <t>https://93mtzf.deta.dev/ticket/378918</t>
         </is>
       </c>
     </row>
@@ -491,11 +491,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>503433</v>
+        <v>835418</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/503433</t>
+          <t>https://93mtzf.deta.dev/ticket/835418</t>
         </is>
       </c>
     </row>
@@ -516,11 +516,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>257987</v>
+        <v>832965</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/257987</t>
+          <t>https://93mtzf.deta.dev/ticket/832965</t>
         </is>
       </c>
     </row>
@@ -541,11 +541,11 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>799241</v>
+        <v>385219</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/799241</t>
+          <t>https://93mtzf.deta.dev/ticket/385219</t>
         </is>
       </c>
     </row>
@@ -566,11 +566,11 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>796294</v>
+        <v>178002</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/796294</t>
+          <t>https://93mtzf.deta.dev/ticket/178002</t>
         </is>
       </c>
     </row>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>184961</v>
+        <v>336085</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/184961</t>
+          <t>https://93mtzf.deta.dev/ticket/336085</t>
         </is>
       </c>
     </row>
@@ -616,11 +616,11 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>502539</v>
+        <v>336491</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/502539</t>
+          <t>https://93mtzf.deta.dev/ticket/336491</t>
         </is>
       </c>
     </row>
@@ -641,31 +641,11 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>929043</v>
+        <v>645991</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/929043</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="D10" t="n">
-        <v>277370</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://93mtzf.deta.dev/ticket/277370</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="D11" t="n">
-        <v>157631</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>https://93mtzf.deta.dev/ticket/157631</t>
+          <t>https://93mtzf.deta.dev/ticket/645991</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
generate qrcode and links for each participant
</commit_message>
<xml_diff>
--- a/assets/Approved_Guests.xlsx
+++ b/assets/Approved_Guests.xlsx
@@ -442,11 +442,11 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>730902</v>
+        <v>868029</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/730902</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/868029</t>
         </is>
       </c>
     </row>
@@ -467,11 +467,11 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>141276</v>
+        <v>467426</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/141276</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/467426</t>
         </is>
       </c>
     </row>
@@ -492,11 +492,11 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>711956</v>
+        <v>209261</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/711956</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/209261</t>
         </is>
       </c>
     </row>
@@ -517,11 +517,11 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>110190</v>
+        <v>116924</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/110190</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/116924</t>
         </is>
       </c>
     </row>
@@ -542,11 +542,11 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>172715</v>
+        <v>119489</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/172715</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/119489</t>
         </is>
       </c>
     </row>
@@ -567,11 +567,11 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>383790</v>
+        <v>558938</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/383790</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/558938</t>
         </is>
       </c>
     </row>
@@ -592,11 +592,11 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>102295</v>
+        <v>820256</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/102295</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/820256</t>
         </is>
       </c>
     </row>
@@ -617,11 +617,11 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>199654</v>
+        <v>667177</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/199654</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/667177</t>
         </is>
       </c>
     </row>
@@ -642,11 +642,11 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>950941</v>
+        <v>829321</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/950941</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/829321</t>
         </is>
       </c>
     </row>
@@ -667,11 +667,11 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>540357</v>
+        <v>230871</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/540357</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/230871</t>
         </is>
       </c>
     </row>
@@ -692,11 +692,11 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>466703</v>
+        <v>894744</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/466703</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/894744</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,11 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>859811</v>
+        <v>129701</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/859811</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/129701</t>
         </is>
       </c>
     </row>
@@ -742,11 +742,11 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>776870</v>
+        <v>206422</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/776870</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/206422</t>
         </is>
       </c>
     </row>
@@ -767,11 +767,11 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>627552</v>
+        <v>210078</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/627552</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/210078</t>
         </is>
       </c>
     </row>
@@ -792,11 +792,11 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>440146</v>
+        <v>555358</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/440146</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/555358</t>
         </is>
       </c>
     </row>
@@ -817,11 +817,11 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>168943</v>
+        <v>679653</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/168943</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/679653</t>
         </is>
       </c>
     </row>
@@ -842,11 +842,11 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>896473</v>
+        <v>942289</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/896473</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/942289</t>
         </is>
       </c>
     </row>
@@ -867,11 +867,11 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>522479</v>
+        <v>784753</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/522479</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/784753</t>
         </is>
       </c>
     </row>
@@ -892,11 +892,11 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>466857</v>
+        <v>751986</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/466857</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/751986</t>
         </is>
       </c>
     </row>
@@ -917,11 +917,11 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>904333</v>
+        <v>823006</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/904333</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/823006</t>
         </is>
       </c>
     </row>
@@ -942,11 +942,11 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>760595</v>
+        <v>296078</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/760595</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/296078</t>
         </is>
       </c>
     </row>
@@ -967,11 +967,11 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>663182</v>
+        <v>869890</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/663182</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/869890</t>
         </is>
       </c>
     </row>
@@ -992,11 +992,11 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>422277</v>
+        <v>418698</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/422277</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/418698</t>
         </is>
       </c>
     </row>
@@ -1017,11 +1017,11 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>930834</v>
+        <v>991458</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/930834</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/991458</t>
         </is>
       </c>
     </row>
@@ -1042,11 +1042,11 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>478606</v>
+        <v>910828</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/478606</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/910828</t>
         </is>
       </c>
     </row>
@@ -1067,11 +1067,11 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>641549</v>
+        <v>724913</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/641549</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/724913</t>
         </is>
       </c>
     </row>
@@ -1092,11 +1092,11 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>605236</v>
+        <v>736647</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/605236</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/736647</t>
         </is>
       </c>
     </row>
@@ -1117,11 +1117,11 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>447921</v>
+        <v>362119</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/447921</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/362119</t>
         </is>
       </c>
     </row>
@@ -1142,11 +1142,11 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>951122</v>
+        <v>826484</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/951122</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/826484</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>472650</v>
+        <v>799912</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>https://93mtzf.deta.dev/ticket/472650</t>
+          <t>https://8000-gaius1-qrcodeticketings-e3bmvm9hf5v.ws-eu102.gitpod.io/ticket/799912</t>
         </is>
       </c>
     </row>

</xml_diff>